<commit_message>
Add another Npc etc
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/DialogueManager/DialogueSheetForm.xlsx
+++ b/Assets/02Script/Manager/DialogueManager/DialogueSheetForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jang\Desktop\GitHubGameProject\RPGGame\Assets\02Script\Manager\DialogueManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0714A21B-0F3F-4FED-AFD4-C009B2B3DB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0063C050-EC33-43A7-8DBB-14A67B8C953B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{CAD4DF56-E29E-41CF-98A8-9E3149639929}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{CAD4DF56-E29E-41CF-98A8-9E3149639929}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,12 +76,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ShouldStopRead</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComfirmBox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Exit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exit</t>
   </si>
 </sst>
 </file>
@@ -445,48 +452,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54781867-1FA7-4C5B-AC3C-22B0018CE468}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92B7F7DB-169A-483B-809C-96394DD3F7F9}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD61DBD6-C33C-4179-9938-23AA7C24BA0F}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B33</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4410726-9782-4B5B-A178-F046F8C273F4}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -516,26 +545,37 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>